<commit_message>
NN-1096 #time 15m bugfix: g2p sample file format issue is solved
</commit_message>
<xml_diff>
--- a/public/Sample-file.xlsx
+++ b/public/Sample-file.xlsx
@@ -137,25 +137,37 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -178,44 +190,44 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="37.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="3" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">

</xml_diff>